<commit_message>
Big commit today. Added in chum salmon and other data. Built time series since 1953
</commit_message>
<xml_diff>
--- a/Data/Keogh_Pink_Salm.xlsx
+++ b/Data/Keogh_Pink_Salm.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylel\OneDrive\Documents\GitHub\Keogh\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAA42434-89B6-4B3F-8B81-1409EA80EF04}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B8A79B-DCD0-40DB-9809-ED75DA96568A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" xr2:uid="{87A42B34-7DA6-45D3-AA8E-381B73CD7DFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021" calcMode="manual"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Year</t>
   </si>
@@ -49,7 +50,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,8 +85,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +108,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,16 +156,26 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma 2" xfId="6" xr:uid="{9BFDFA3D-EE83-4630-9A2B-9EC4C5FC632D}"/>
@@ -470,19 +499,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB21D5EE-6061-4061-ABBA-3CA749FC0B73}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="10"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -490,255 +522,503 @@
       <c r="A2" s="1">
         <v>2015</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>6600</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B3" s="2">
-        <v>78943</v>
+        <v>2014</v>
+      </c>
+      <c r="B3" s="5">
+        <v>801476</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2011</v>
-      </c>
-      <c r="B4" s="2">
-        <v>4530</v>
+        <v>2013</v>
+      </c>
+      <c r="B4" s="3">
+        <v>78943</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B5" s="2">
-        <v>22308</v>
+        <v>2012</v>
+      </c>
+      <c r="B5" s="5">
+        <v>84500</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>2007</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5189</v>
+        <v>2011</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4530</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>2005</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3134</v>
+        <v>2010</v>
+      </c>
+      <c r="B7" s="5">
+        <v>9308</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2003</v>
-      </c>
-      <c r="B8" s="2">
-        <v>4771</v>
+        <v>2009</v>
+      </c>
+      <c r="B8" s="3">
+        <v>22308</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>2001</v>
-      </c>
-      <c r="B9" s="3">
-        <v>3838</v>
+        <v>2008</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3175</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1999</v>
-      </c>
-      <c r="B10" s="4">
-        <v>860</v>
+        <v>2007</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5189</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1997</v>
-      </c>
-      <c r="B11" s="4">
-        <v>75</v>
+        <v>2006</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10926</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1995</v>
-      </c>
-      <c r="B12" s="4">
-        <v>350</v>
+        <v>2005</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3134</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1993</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>2</v>
+        <v>2004</v>
+      </c>
+      <c r="B13" s="6">
+        <v>84200</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1991</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>2</v>
+        <v>2003</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4771</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1989</v>
-      </c>
-      <c r="B15" s="4">
-        <v>330</v>
+        <v>2002</v>
+      </c>
+      <c r="B15" s="7">
+        <v>107697</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1987</v>
-      </c>
-      <c r="B16" s="4">
-        <v>700</v>
+        <v>2001</v>
+      </c>
+      <c r="B16" s="2">
+        <v>3838</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1985</v>
-      </c>
-      <c r="B17" s="4">
-        <v>32650</v>
+        <v>2000</v>
+      </c>
+      <c r="B17" s="7">
+        <v>25529</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1983</v>
-      </c>
-      <c r="B18" s="4">
-        <v>15000</v>
+        <v>1999</v>
+      </c>
+      <c r="B18" s="3">
+        <v>860</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1981</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>2</v>
+        <v>1998</v>
+      </c>
+      <c r="B19" s="8">
+        <v>10100</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1979</v>
-      </c>
-      <c r="B20" s="4">
-        <v>200</v>
+        <v>1997</v>
+      </c>
+      <c r="B20" s="3">
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1977</v>
-      </c>
-      <c r="B21" s="4">
-        <v>2100</v>
+        <v>1996</v>
+      </c>
+      <c r="B21" s="8">
+        <v>15000</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1975</v>
-      </c>
-      <c r="B22" s="4">
-        <v>2500</v>
+        <v>1995</v>
+      </c>
+      <c r="B22" s="3">
+        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1973</v>
-      </c>
-      <c r="B23" s="4">
-        <v>7000</v>
+        <v>1994</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1971</v>
-      </c>
-      <c r="B24" s="4">
-        <v>3500</v>
+        <v>1993</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1969</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1500</v>
+        <v>1992</v>
+      </c>
+      <c r="B25" s="9">
+        <v>80000</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1967</v>
-      </c>
-      <c r="B26" s="4">
-        <v>3500</v>
+        <v>1991</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1965</v>
-      </c>
-      <c r="B27" s="4">
+        <v>1990</v>
+      </c>
+      <c r="B27" s="9">
         <v>15000</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1963</v>
-      </c>
-      <c r="B28" s="4">
-        <v>7500</v>
+        <v>1989</v>
+      </c>
+      <c r="B28" s="3">
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>1961</v>
-      </c>
-      <c r="B29" s="4">
-        <v>15000</v>
+        <v>1988</v>
+      </c>
+      <c r="B29" s="9">
+        <v>50000</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1959</v>
-      </c>
-      <c r="B30" s="4">
-        <v>35000</v>
+        <v>1987</v>
+      </c>
+      <c r="B30" s="3">
+        <v>700</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>1957</v>
-      </c>
-      <c r="B31" s="4">
-        <v>35000</v>
+        <v>1986</v>
+      </c>
+      <c r="B31" s="9">
+        <v>100000</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>1955</v>
-      </c>
-      <c r="B32" s="4">
-        <v>7500</v>
+        <v>1985</v>
+      </c>
+      <c r="B32" s="3">
+        <v>32650</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
+        <v>1984</v>
+      </c>
+      <c r="B33" s="9">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>1983</v>
+      </c>
+      <c r="B34" s="3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>1982</v>
+      </c>
+      <c r="B35" s="9">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>1981</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>1980</v>
+      </c>
+      <c r="B37" s="9">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>1979</v>
+      </c>
+      <c r="B38" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>1978</v>
+      </c>
+      <c r="B39" s="9">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>1977</v>
+      </c>
+      <c r="B40" s="3">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>1976</v>
+      </c>
+      <c r="B41" s="9">
+        <v>72000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>1975</v>
+      </c>
+      <c r="B42" s="3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1974</v>
+      </c>
+      <c r="B43" s="9">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>1973</v>
+      </c>
+      <c r="B44" s="3">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>1972</v>
+      </c>
+      <c r="B45" s="9">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>1971</v>
+      </c>
+      <c r="B46" s="3">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>1970</v>
+      </c>
+      <c r="B47" s="9">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>1969</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>1968</v>
+      </c>
+      <c r="B49" s="9">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>1967</v>
+      </c>
+      <c r="B50" s="3">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>1966</v>
+      </c>
+      <c r="B51" s="9">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>1965</v>
+      </c>
+      <c r="B52" s="3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>1964</v>
+      </c>
+      <c r="B53" s="9">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>1963</v>
+      </c>
+      <c r="B54" s="3">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>1962</v>
+      </c>
+      <c r="B55" s="9">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>1961</v>
+      </c>
+      <c r="B56" s="3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>1960</v>
+      </c>
+      <c r="B57" s="9">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>1959</v>
+      </c>
+      <c r="B58" s="3">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>1958</v>
+      </c>
+      <c r="B59" s="9">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>1957</v>
+      </c>
+      <c r="B60" s="3">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>1956</v>
+      </c>
+      <c r="B61" s="9">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>1955</v>
+      </c>
+      <c r="B62" s="3">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>1954</v>
+      </c>
+      <c r="B63" s="9">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>1953</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B64" s="3">
         <v>7500</v>
       </c>
     </row>

</xml_diff>